<commit_message>
add a rentals comp doc
</commit_message>
<xml_diff>
--- a/docs/30315 rentals zillow.csv.xlsx
+++ b/docs/30315 rentals zillow.csv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f65a642d0762be/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f65a642d0762be/Desktop/214_assets/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A5B003B-8ADB-4BF8-912F-05D3F6DF4E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{3A5B003B-8ADB-4BF8-912F-05D3F6DF4E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C375929-FFF9-41E2-B68C-F6EC50B8AC9B}"/>
   <bookViews>
-    <workbookView xWindow="3252" yWindow="0" windowWidth="20004" windowHeight="12240" xr2:uid="{2B16E20F-E0B2-4595-8A4C-E19F2E68991D}"/>
+    <workbookView xWindow="2124" yWindow="600" windowWidth="20004" windowHeight="11640" xr2:uid="{2B16E20F-E0B2-4595-8A4C-E19F2E68991D}"/>
   </bookViews>
   <sheets>
     <sheet name="zillow (7)" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +565,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -728,9 +734,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1106,32 +1113,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE30E02B-F752-4BE7-80D0-C00AD466B578}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1142,7 +1154,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1153,7 +1165,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1176,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1186,7 +1198,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1200,7 +1212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1214,7 +1226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1228,7 +1240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1256,7 +1268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +1282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1284,7 +1296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1312,7 +1324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>

</xml_diff>